<commit_message>
added pushups for last day in october
</commit_message>
<xml_diff>
--- a/Workout_2020.xlsx
+++ b/Workout_2020.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tepavceb\Documents\My workouts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workout-diary\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="June" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="64">
   <si>
     <t>kb swings</t>
   </si>
@@ -197,9 +197,6 @@
     <t>10 x 8 - 44lb</t>
   </si>
   <si>
-    <t>5 x ?</t>
-  </si>
-  <si>
     <t>23 x 9</t>
   </si>
   <si>
@@ -219,6 +216,12 @@
   </si>
   <si>
     <t>10 x 10 - 44lb</t>
+  </si>
+  <si>
+    <t>23 x 6</t>
+  </si>
+  <si>
+    <t>6 x ?</t>
   </si>
 </sst>
 </file>
@@ -1619,8 +1622,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AKX34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1803,7 +1806,7 @@
         <v>44125</v>
       </c>
       <c r="C22" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K22">
         <v>207</v>
@@ -2838,7 +2841,7 @@
         <v>44131</v>
       </c>
       <c r="C28" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K28">
         <v>230</v>
@@ -2860,7 +2863,7 @@
         <v>44133</v>
       </c>
       <c r="B30" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K30">
         <v>160</v>
@@ -2871,7 +2874,7 @@
         <v>44134</v>
       </c>
       <c r="G31" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K31">
         <v>100</v>
@@ -2882,7 +2885,10 @@
         <v>44135</v>
       </c>
       <c r="C32" t="s">
-        <v>58</v>
+        <v>62</v>
+      </c>
+      <c r="K32">
+        <v>138</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
@@ -2894,6 +2900,9 @@
       </c>
       <c r="B34">
         <v>460</v>
+      </c>
+      <c r="C34">
+        <v>575</v>
       </c>
       <c r="E34">
         <v>50</v>
@@ -2912,8 +2921,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2969,7 +2978,7 @@
         <v>44137</v>
       </c>
       <c r="E3" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -2977,7 +2986,7 @@
         <v>44138</v>
       </c>
       <c r="B4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -2985,7 +2994,7 @@
         <v>44139</v>
       </c>
       <c r="G5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -2993,7 +3002,7 @@
         <v>44140</v>
       </c>
       <c r="C6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -3001,7 +3010,7 @@
         <v>44141</v>
       </c>
       <c r="E7" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -3009,7 +3018,7 @@
         <v>44142</v>
       </c>
       <c r="B8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -3032,7 +3041,7 @@
         <v>44144</v>
       </c>
       <c r="G10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -3040,7 +3049,7 @@
         <v>44145</v>
       </c>
       <c r="C11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -3048,7 +3057,7 @@
         <v>44146</v>
       </c>
       <c r="E12" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -3056,7 +3065,7 @@
         <v>44147</v>
       </c>
       <c r="B13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -3064,7 +3073,7 @@
         <v>44148</v>
       </c>
       <c r="G14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -3072,7 +3081,7 @@
         <v>44149</v>
       </c>
       <c r="C15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -3095,7 +3104,7 @@
         <v>44151</v>
       </c>
       <c r="E17" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
@@ -3103,7 +3112,7 @@
         <v>44152</v>
       </c>
       <c r="B18" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
@@ -3111,7 +3120,7 @@
         <v>44153</v>
       </c>
       <c r="G19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
@@ -3119,7 +3128,7 @@
         <v>44154</v>
       </c>
       <c r="C20" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
@@ -3127,7 +3136,7 @@
         <v>44155</v>
       </c>
       <c r="E21" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
@@ -3135,7 +3144,7 @@
         <v>44156</v>
       </c>
       <c r="B22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
@@ -3158,7 +3167,7 @@
         <v>44158</v>
       </c>
       <c r="G24" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
@@ -3166,7 +3175,7 @@
         <v>44159</v>
       </c>
       <c r="C25" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
@@ -3174,7 +3183,7 @@
         <v>44160</v>
       </c>
       <c r="E26" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
@@ -3182,7 +3191,7 @@
         <v>44161</v>
       </c>
       <c r="B27" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
@@ -3190,7 +3199,7 @@
         <v>44162</v>
       </c>
       <c r="G28" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
@@ -3198,7 +3207,7 @@
         <v>44163</v>
       </c>
       <c r="C29" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
@@ -3221,7 +3230,7 @@
         <v>44165</v>
       </c>
       <c r="E31" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
week of November 2
</commit_message>
<xml_diff>
--- a/Workout_2020.xlsx
+++ b/Workout_2020.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="68">
   <si>
     <t>kb swings</t>
   </si>
@@ -221,7 +221,19 @@
     <t>23 x 6</t>
   </si>
   <si>
-    <t>6 x ?</t>
+    <t>6 x 9</t>
+  </si>
+  <si>
+    <t>20 x 10 - 53lb</t>
+  </si>
+  <si>
+    <t>10 x 9 - 44lb</t>
+  </si>
+  <si>
+    <t>6 x 11</t>
+  </si>
+  <si>
+    <t>7 x ?</t>
   </si>
 </sst>
 </file>
@@ -1622,8 +1634,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AKX34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2922,7 +2934,7 @@
   <dimension ref="A1:K33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2980,13 +2992,19 @@
       <c r="E3" t="s">
         <v>63</v>
       </c>
+      <c r="K3">
+        <v>54</v>
+      </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>44138</v>
       </c>
       <c r="B4" t="s">
-        <v>58</v>
+        <v>64</v>
+      </c>
+      <c r="K4">
+        <v>200</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -2994,7 +3012,10 @@
         <v>44139</v>
       </c>
       <c r="G5" t="s">
-        <v>59</v>
+        <v>65</v>
+      </c>
+      <c r="K5">
+        <v>90</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -3002,7 +3023,10 @@
         <v>44140</v>
       </c>
       <c r="C6" t="s">
-        <v>57</v>
+        <v>56</v>
+      </c>
+      <c r="K6">
+        <v>230</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -3010,7 +3034,10 @@
         <v>44141</v>
       </c>
       <c r="E7" t="s">
-        <v>63</v>
+        <v>66</v>
+      </c>
+      <c r="K7">
+        <v>66</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -3057,7 +3084,7 @@
         <v>44146</v>
       </c>
       <c r="E12" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -3104,7 +3131,7 @@
         <v>44151</v>
       </c>
       <c r="E17" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
@@ -3136,7 +3163,7 @@
         <v>44155</v>
       </c>
       <c r="E21" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
@@ -3183,7 +3210,7 @@
         <v>44160</v>
       </c>
       <c r="E26" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
@@ -3230,7 +3257,7 @@
         <v>44165</v>
       </c>
       <c r="E31" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>